<commit_message>
feat: added error handling of input data
</commit_message>
<xml_diff>
--- a/Data/Output/Sales List.xlsx
+++ b/Data/Output/Sales List.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:O30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -474,6 +474,41 @@
           <t>TOTAL PRICE</t>
         </is>
       </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Unit Cost (BRL)</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Total Price (BRL)</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Exchange Conversion Date/Time</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Address</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Neighborhood</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Location/State</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>ERRORS_FOUND</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -516,6 +551,13 @@
           <t>246318 USD</t>
         </is>
       </c>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -558,6 +600,13 @@
           <t>204472 EUR</t>
         </is>
       </c>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -600,6 +649,13 @@
           <t>133375 RON</t>
         </is>
       </c>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -642,6 +698,13 @@
           <t>203623 USD</t>
         </is>
       </c>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -684,6 +747,13 @@
           <t>5155 RON</t>
         </is>
       </c>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -726,6 +796,13 @@
           <t>88032 EUR</t>
         </is>
       </c>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -768,6 +845,13 @@
           <t>83007 RON</t>
         </is>
       </c>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -810,6 +894,13 @@
           <t>101118 EUR</t>
         </is>
       </c>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -852,6 +943,13 @@
           <t>62685 EUR</t>
         </is>
       </c>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -894,6 +992,13 @@
           <t>199584 EUR</t>
         </is>
       </c>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
+      <c r="O11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -936,6 +1041,13 @@
           <t>286085 USD</t>
         </is>
       </c>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr"/>
+      <c r="O12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -978,6 +1090,13 @@
           <t>328950 EUR</t>
         </is>
       </c>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr"/>
+      <c r="O13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1020,6 +1139,13 @@
           <t>19576 USD</t>
         </is>
       </c>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr"/>
+      <c r="L14" t="inlineStr"/>
+      <c r="M14" t="inlineStr"/>
+      <c r="N14" t="inlineStr"/>
+      <c r="O14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1062,6 +1188,13 @@
           <t>358200 CAD</t>
         </is>
       </c>
+      <c r="I15" t="inlineStr"/>
+      <c r="J15" t="inlineStr"/>
+      <c r="K15" t="inlineStr"/>
+      <c r="L15" t="inlineStr"/>
+      <c r="M15" t="inlineStr"/>
+      <c r="N15" t="inlineStr"/>
+      <c r="O15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1104,6 +1237,13 @@
           <t>332614 USD</t>
         </is>
       </c>
+      <c r="I16" t="inlineStr"/>
+      <c r="J16" t="inlineStr"/>
+      <c r="K16" t="inlineStr"/>
+      <c r="L16" t="inlineStr"/>
+      <c r="M16" t="inlineStr"/>
+      <c r="N16" t="inlineStr"/>
+      <c r="O16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1146,6 +1286,13 @@
           <t>186975 USD</t>
         </is>
       </c>
+      <c r="I17" t="inlineStr"/>
+      <c r="J17" t="inlineStr"/>
+      <c r="K17" t="inlineStr"/>
+      <c r="L17" t="inlineStr"/>
+      <c r="M17" t="inlineStr"/>
+      <c r="N17" t="inlineStr"/>
+      <c r="O17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1188,6 +1335,13 @@
           <t>298040 EUR</t>
         </is>
       </c>
+      <c r="I18" t="inlineStr"/>
+      <c r="J18" t="inlineStr"/>
+      <c r="K18" t="inlineStr"/>
+      <c r="L18" t="inlineStr"/>
+      <c r="M18" t="inlineStr"/>
+      <c r="N18" t="inlineStr"/>
+      <c r="O18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1230,6 +1384,13 @@
           <t>48072 RON</t>
         </is>
       </c>
+      <c r="I19" t="inlineStr"/>
+      <c r="J19" t="inlineStr"/>
+      <c r="K19" t="inlineStr"/>
+      <c r="L19" t="inlineStr"/>
+      <c r="M19" t="inlineStr"/>
+      <c r="N19" t="inlineStr"/>
+      <c r="O19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1272,6 +1433,13 @@
           <t>180900 RON</t>
         </is>
       </c>
+      <c r="I20" t="inlineStr"/>
+      <c r="J20" t="inlineStr"/>
+      <c r="K20" t="inlineStr"/>
+      <c r="L20" t="inlineStr"/>
+      <c r="M20" t="inlineStr"/>
+      <c r="N20" t="inlineStr"/>
+      <c r="O20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1314,6 +1482,13 @@
           <t>141872 USD</t>
         </is>
       </c>
+      <c r="I21" t="inlineStr"/>
+      <c r="J21" t="inlineStr"/>
+      <c r="K21" t="inlineStr"/>
+      <c r="L21" t="inlineStr"/>
+      <c r="M21" t="inlineStr"/>
+      <c r="N21" t="inlineStr"/>
+      <c r="O21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1356,6 +1531,13 @@
           <t>343728 USD</t>
         </is>
       </c>
+      <c r="I22" t="inlineStr"/>
+      <c r="J22" t="inlineStr"/>
+      <c r="K22" t="inlineStr"/>
+      <c r="L22" t="inlineStr"/>
+      <c r="M22" t="inlineStr"/>
+      <c r="N22" t="inlineStr"/>
+      <c r="O22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1398,6 +1580,13 @@
           <t>113412 USD</t>
         </is>
       </c>
+      <c r="I23" t="inlineStr"/>
+      <c r="J23" t="inlineStr"/>
+      <c r="K23" t="inlineStr"/>
+      <c r="L23" t="inlineStr"/>
+      <c r="M23" t="inlineStr"/>
+      <c r="N23" t="inlineStr"/>
+      <c r="O23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1440,6 +1629,13 @@
           <t>284837 RON</t>
         </is>
       </c>
+      <c r="I24" t="inlineStr"/>
+      <c r="J24" t="inlineStr"/>
+      <c r="K24" t="inlineStr"/>
+      <c r="L24" t="inlineStr"/>
+      <c r="M24" t="inlineStr"/>
+      <c r="N24" t="inlineStr"/>
+      <c r="O24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1482,6 +1678,13 @@
           <t>77520 EUR</t>
         </is>
       </c>
+      <c r="I25" t="inlineStr"/>
+      <c r="J25" t="inlineStr"/>
+      <c r="K25" t="inlineStr"/>
+      <c r="L25" t="inlineStr"/>
+      <c r="M25" t="inlineStr"/>
+      <c r="N25" t="inlineStr"/>
+      <c r="O25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1524,6 +1727,13 @@
           <t>227946 FJD</t>
         </is>
       </c>
+      <c r="I26" t="inlineStr"/>
+      <c r="J26" t="inlineStr"/>
+      <c r="K26" t="inlineStr"/>
+      <c r="L26" t="inlineStr"/>
+      <c r="M26" t="inlineStr"/>
+      <c r="N26" t="inlineStr"/>
+      <c r="O26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1566,6 +1776,13 @@
           <t>184923 EUR</t>
         </is>
       </c>
+      <c r="I27" t="inlineStr"/>
+      <c r="J27" t="inlineStr"/>
+      <c r="K27" t="inlineStr"/>
+      <c r="L27" t="inlineStr"/>
+      <c r="M27" t="inlineStr"/>
+      <c r="N27" t="inlineStr"/>
+      <c r="O27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1608,6 +1825,13 @@
           <t>176729 EUR</t>
         </is>
       </c>
+      <c r="I28" t="inlineStr"/>
+      <c r="J28" t="inlineStr"/>
+      <c r="K28" t="inlineStr"/>
+      <c r="L28" t="inlineStr"/>
+      <c r="M28" t="inlineStr"/>
+      <c r="N28" t="inlineStr"/>
+      <c r="O28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1650,6 +1874,13 @@
           <t>2 BTC</t>
         </is>
       </c>
+      <c r="I29" t="inlineStr"/>
+      <c r="J29" t="inlineStr"/>
+      <c r="K29" t="inlineStr"/>
+      <c r="L29" t="inlineStr"/>
+      <c r="M29" t="inlineStr"/>
+      <c r="N29" t="inlineStr"/>
+      <c r="O29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1692,6 +1923,13 @@
           <t>175050 USD</t>
         </is>
       </c>
+      <c r="I30" t="inlineStr"/>
+      <c r="J30" t="inlineStr"/>
+      <c r="K30" t="inlineStr"/>
+      <c r="L30" t="inlineStr"/>
+      <c r="M30" t="inlineStr"/>
+      <c r="N30" t="inlineStr"/>
+      <c r="O30" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
feat: added vba code to format pdf and added password to pdf
</commit_message>
<xml_diff>
--- a/Data/Output/Sales List.xlsx
+++ b/Data/Output/Sales List.xlsx
@@ -553,17 +553,17 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>227179.091400</t>
+          <t>41053</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>1363074.548400</t>
+          <t>246318</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>02/08/2025</t>
+          <t>05/08/2025</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
@@ -626,17 +626,17 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>163944.8828300</t>
+          <t>25559</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>1311559.0626400</t>
+          <t>204472</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>02/08/2025</t>
+          <t>05/08/2025</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
@@ -699,17 +699,17 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>33721.3412937500</t>
+          <t>26675</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>168606.7064687500</t>
+          <t>133375</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>02/08/2025</t>
+          <t>05/08/2025</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
@@ -772,17 +772,17 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>160972.708200</t>
+          <t>29089</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>1126808.957400</t>
+          <t>203623</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>02/08/2025</t>
+          <t>05/08/2025</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
@@ -845,17 +845,17 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>1303.3440627500</t>
+          <t>1031</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>6516.7203137500</t>
+          <t>5155</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>02/08/2025</t>
+          <t>05/08/2025</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
@@ -922,17 +922,17 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>70583.7274800</t>
+          <t>11004</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>564669.8198400</t>
+          <t>88032</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>02/08/2025</t>
+          <t>05/08/2025</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
@@ -995,17 +995,17 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>11659.3038707500</t>
+          <t>9223</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>104933.7348367500</t>
+          <t>83007</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>02/08/2025</t>
+          <t>05/08/2025</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
@@ -1072,17 +1072,17 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>216202.7552200</t>
+          <t>33706</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>648608.2656600</t>
+          <t>101118</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>02/08/2025</t>
+          <t>05/08/2025</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
@@ -1149,17 +1149,17 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>57440.6833500</t>
+          <t>8955</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>402084.7834500</t>
+          <t>62685</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>02/08/2025</t>
+          <t>05/08/2025</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
@@ -1222,17 +1222,17 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>160025.7027600</t>
+          <t>24948</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>1280205.6220800</t>
+          <t>199584</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>02/08/2025</t>
+          <t>05/08/2025</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
@@ -1295,17 +1295,17 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>316627.434600</t>
+          <t>57217</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>1583137.173000</t>
+          <t>286085</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>02/08/2025</t>
+          <t>05/08/2025</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
@@ -1368,17 +1368,17 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>211000.7011500</t>
+          <t>32895</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>2110007.0115000</t>
+          <t>328950</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>02/08/2025</t>
+          <t>05/08/2025</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
@@ -1441,17 +1441,17 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>13541.208600</t>
+          <t>2447</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>108329.668800</t>
+          <t>19576</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>02/08/2025</t>
+          <t>05/08/2025</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
@@ -1514,17 +1514,17 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>159777.100000</t>
+          <t>39800</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>1437993.900000</t>
+          <t>358200</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>02/08/2025</t>
+          <t>05/08/2025</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
@@ -1591,17 +1591,17 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>1840619.353200</t>
+          <t>332614</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>1840619.353200</t>
+          <t>332614</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>02/08/2025</t>
+          <t>05/08/2025</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
@@ -1664,17 +1664,17 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>114964.695000</t>
+          <t>20775</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>1034682.255000</t>
+          <t>186975</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>02/08/2025</t>
+          <t>05/08/2025</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
@@ -1741,17 +1741,17 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>238967.3543500</t>
+          <t>37255</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>1911738.8348000</t>
+          <t>298040</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>02/08/2025</t>
+          <t>05/08/2025</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
@@ -1814,17 +1814,17 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>30385.2355890000</t>
+          <t>24036</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>60770.4711780000</t>
+          <t>48072</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>02/08/2025</t>
+          <t>05/08/2025</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
@@ -1891,17 +1891,17 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>22868.5684725000</t>
+          <t>18090</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>228685.6847250000</t>
+          <t>180900</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>02/08/2025</t>
+          <t>05/08/2025</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
@@ -1964,17 +1964,17 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>98136.409200</t>
+          <t>17734</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>785091.273600</t>
+          <t>141872</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>02/08/2025</t>
+          <t>05/08/2025</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
@@ -2037,17 +2037,17 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>211346.889600</t>
+          <t>38192</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>1902122.006400</t>
+          <t>343728</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>02/08/2025</t>
+          <t>05/08/2025</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
@@ -2114,17 +2114,17 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>104599.887600</t>
+          <t>18902</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>627599.325600</t>
+          <t>113412</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>02/08/2025</t>
+          <t>05/08/2025</t>
         </is>
       </c>
       <c r="L23" t="inlineStr">
@@ -2187,17 +2187,17 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>51439.7412777500</t>
+          <t>40691</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>360078.1889442500</t>
+          <t>284837</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>02/08/2025</t>
+          <t>05/08/2025</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">
@@ -2264,17 +2264,17 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>49724.1962400</t>
+          <t>7752</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>497241.9624000</t>
+          <t>77520</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>02/08/2025</t>
+          <t>05/08/2025</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
@@ -2339,7 +2339,7 @@
       <c r="J26" t="inlineStr"/>
       <c r="K26" t="inlineStr">
         <is>
-          <t>02/08/2025</t>
+          <t>05/08/2025</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
@@ -2406,17 +2406,17 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>131796.0603900</t>
+          <t>20547</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>1186164.5435100</t>
+          <t>184923</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>02/08/2025</t>
+          <t>05/08/2025</t>
         </is>
       </c>
       <c r="L27" t="inlineStr">
@@ -2479,17 +2479,17 @@
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>1133605.1957300</t>
+          <t>176729</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>1133605.1957300</t>
+          <t>176729</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>02/08/2025</t>
+          <t>05/08/2025</t>
         </is>
       </c>
       <c r="L28" t="inlineStr">
@@ -2552,17 +2552,17 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>1256600.00</t>
+          <t>2</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>1256600.00</t>
+          <t>2</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>02/08/2025</t>
+          <t>05/08/2025</t>
         </is>
       </c>
       <c r="L29" t="inlineStr">
@@ -2625,17 +2625,17 @@
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>107632.410000</t>
+          <t>19450</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>968691.690000</t>
+          <t>175050</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>02/08/2025</t>
+          <t>05/08/2025</t>
         </is>
       </c>
       <c r="L30" t="inlineStr">

</xml_diff>